<commit_message>
add readme.txt for influxdb docker
</commit_message>
<xml_diff>
--- a/doc/P4J_BCM_Match.xlsx
+++ b/doc/P4J_BCM_Match.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Personal\Projects\Programming\AutomationServer\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{3E2C5E70-A1BD-407D-9E3F-843A213933C1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{BBB0D829-239B-48FA-B9AE-DF3F16C215CA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -453,7 +453,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>